<commit_message>
update readme with picture
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -24,13 +24,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>項目</t>
+    <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>日期</t>
+    <t>結婚紀念日</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -38,11 +38,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>結婚紀念日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxx</t>
+    <t>項目名稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -51,9 +47,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="180" formatCode="mm/dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +64,13 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Adobe 繁黑體 Std B"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,11 +95,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -379,52 +385,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2"/>
+    <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44638</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44690</v>
-      </c>
-      <c r="C3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44692</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>